<commit_message>
Update to levee setback and levee removal codes
Mostly work updating the results plotting
</commit_message>
<xml_diff>
--- a/Projects/Oneto_Denier/mf_wb_color_dict.xlsx
+++ b/Projects/Oneto_Denier/mf_wb_color_dict.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrewc\Documents\GitHub\CosumnesRiverRecharge\Projects\Oneto_Denier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9653DD3F-3A1C-4965-857F-FBE9E1B7BDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5003FD-90F8-424B-986A-9D6EC020EB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mf_wb_dict" sheetId="1" r:id="rId1"/>
     <sheet name="owhm_wb_dict" sheetId="2" r:id="rId2"/>
+    <sheet name="flopy_to_owhm" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="78">
   <si>
     <t># general color correspondance for zone budget plotting in matplotlib.pyplot using a dictionary</t>
   </si>
@@ -234,6 +235,27 @@
   </si>
   <si>
     <t>Floodplain Discharge</t>
+  </si>
+  <si>
+    <t>flopy</t>
+  </si>
+  <si>
+    <t>owhm</t>
+  </si>
+  <si>
+    <t>GHB_IN</t>
+  </si>
+  <si>
+    <t>GHB_OUT</t>
+  </si>
+  <si>
+    <t># dictionary matching flopy wb summary to flopy zonebudget naming (GW_IN is a manual addition)</t>
+  </si>
+  <si>
+    <t>dSTORAGE_sum</t>
+  </si>
+  <si>
+    <t>Cumulative Storage Change</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1099,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1350,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1476,6 +1498,167 @@
         <v>70</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B4F636-09E4-469D-B011-A25B59359DC7}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates to regional model and economic irrigation model
</commit_message>
<xml_diff>
--- a/Projects/Oneto_Denier/mf_wb_color_dict.xlsx
+++ b/Projects/Oneto_Denier/mf_wb_color_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrewc\Documents\GitHub\CosumnesRiverRecharge\Projects\Oneto_Denier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5003FD-90F8-424B-986A-9D6EC020EB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BB92D6-C14F-4A05-9BC2-993BEE0DF5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mf_wb_dict" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
   <si>
     <t># general color correspondance for zone budget plotting in matplotlib.pyplot using a dictionary</t>
   </si>
@@ -210,9 +210,6 @@
     <t>LAK_OUT</t>
   </si>
   <si>
-    <t>Stream Leakage</t>
-  </si>
-  <si>
     <t>Baseflow</t>
   </si>
   <si>
@@ -256,6 +253,15 @@
   </si>
   <si>
     <t>Cumulative Storage Change</t>
+  </si>
+  <si>
+    <t>GHB_NET</t>
+  </si>
+  <si>
+    <t>Net Groundwater Flow</t>
+  </si>
+  <si>
+    <t>Stream Recharge</t>
   </si>
 </sst>
 </file>
@@ -1372,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1404,7 +1410,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1415,10 +1421,10 @@
         <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1426,10 +1432,10 @@
         <v>55</v>
       </c>
       <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
         <v>66</v>
-      </c>
-      <c r="C5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1440,7 +1446,7 @@
         <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1470,10 +1476,10 @@
         <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1484,7 +1490,7 @@
         <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1492,43 +1498,54 @@
         <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
         <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
       </c>
       <c r="C14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>77</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1540,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B4F636-09E4-469D-B011-A25B59359DC7}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1552,15 +1569,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1637,7 +1654,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
@@ -1645,7 +1662,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
@@ -1653,10 +1670,10 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on levee removal scripts
</commit_message>
<xml_diff>
--- a/Projects/Oneto_Denier/mf_wb_color_dict.xlsx
+++ b/Projects/Oneto_Denier/mf_wb_color_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrewc\Documents\GitHub\CosumnesRiverRecharge\Projects\Oneto_Denier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BB92D6-C14F-4A05-9BC2-993BEE0DF5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B722386-971B-4A0F-BD4B-6FCB106593D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="82">
   <si>
     <t># general color correspondance for zone budget plotting in matplotlib.pyplot using a dictionary</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>Stream Recharge</t>
+  </si>
+  <si>
+    <t>name_old</t>
+  </si>
+  <si>
+    <t>Stream Losses</t>
   </si>
 </sst>
 </file>
@@ -1378,23 +1384,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="3" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1404,8 +1411,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1415,8 +1425,11 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1424,10 +1437,13 @@
         <v>64</v>
       </c>
       <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1437,8 +1453,11 @@
       <c r="C5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1448,8 +1467,11 @@
       <c r="C6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1459,8 +1481,11 @@
       <c r="C7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1470,8 +1495,11 @@
       <c r="C8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1481,8 +1509,11 @@
       <c r="C9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -1492,8 +1523,11 @@
       <c r="C10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1503,8 +1537,11 @@
       <c r="C11" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1514,8 +1551,11 @@
       <c r="C12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -1525,8 +1565,11 @@
       <c r="C13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -1536,8 +1579,11 @@
       <c r="C14" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -1545,6 +1591,9 @@
         <v>44</v>
       </c>
       <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Stream seepage plotting udpates
Improve parallel output plotting
</commit_message>
<xml_diff>
--- a/Projects/Oneto_Denier/mf_wb_color_dict.xlsx
+++ b/Projects/Oneto_Denier/mf_wb_color_dict.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrewc\Documents\GitHub\CosumnesRiverRecharge\Projects\Oneto_Denier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajcalder\Documents\GitHub\CosumnesRiverRecharge\Projects\Oneto_Denier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B722386-971B-4A0F-BD4B-6FCB106593D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C629C0AB-46E1-4C5C-A9F0-51A6A66AD0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mf_wb_dict" sheetId="1" r:id="rId1"/>
     <sheet name="owhm_wb_dict" sheetId="2" r:id="rId2"/>
     <sheet name="flopy_to_owhm" sheetId="3" r:id="rId3"/>
+    <sheet name="plt_ref" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="93">
   <si>
     <t># general color correspondance for zone budget plotting in matplotlib.pyplot using a dictionary</t>
   </si>
@@ -268,6 +269,39 @@
   </si>
   <si>
     <t>Stream Losses</t>
+  </si>
+  <si>
+    <t># other useful name referencing based on project specific naming</t>
+  </si>
+  <si>
+    <t>Qbase</t>
+  </si>
+  <si>
+    <t>Qrech</t>
+  </si>
+  <si>
+    <t>flowing</t>
+  </si>
+  <si>
+    <t>Qout</t>
+  </si>
+  <si>
+    <t>No. Days with Flow</t>
+  </si>
+  <si>
+    <t>Streamflow</t>
+  </si>
+  <si>
+    <t>num_sfr_coarse</t>
+  </si>
+  <si>
+    <t>num_lak_coarse</t>
+  </si>
+  <si>
+    <t>No. of Coarse Reaches</t>
+  </si>
+  <si>
+    <t>No. of Coarse Lake Cells</t>
   </si>
 </sst>
 </file>
@@ -1114,17 +1148,17 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1135,7 +1169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1146,7 +1180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1157,7 +1191,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1168,7 +1202,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1179,7 +1213,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1190,7 +1224,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1201,7 +1235,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1212,7 +1246,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1223,7 +1257,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1234,7 +1268,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1245,7 +1279,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1256,7 +1290,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1267,7 +1301,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1278,7 +1312,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1289,7 +1323,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1300,7 +1334,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1311,7 +1345,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1322,7 +1356,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1333,7 +1367,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1344,7 +1378,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1355,7 +1389,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -1366,7 +1400,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -1386,22 +1420,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="3" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="3" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1415,7 +1449,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1429,7 +1463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1443,7 +1477,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1457,7 +1491,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1471,7 +1505,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1485,7 +1519,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1499,7 +1533,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1513,7 +1547,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -1527,7 +1561,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1541,7 +1575,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1555,7 +1589,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -1569,7 +1603,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -1583,7 +1617,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -1610,18 +1644,18 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -1629,7 +1663,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1637,7 +1671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1645,7 +1679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1653,7 +1687,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1661,7 +1695,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1669,7 +1703,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1677,7 +1711,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1685,7 +1719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -1693,7 +1727,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1701,7 +1735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1709,7 +1743,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -1717,12 +1751,91 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>75</v>
       </c>
       <c r="B14" t="s">
         <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A5EE0D-BF41-4D68-8FFD-ABD893E02549}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>